<commit_message>
Finalized string_generator excel file. Working firmware for process control.
</commit_message>
<xml_diff>
--- a/string_generator.xlsx
+++ b/string_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/kasper_arizona_edu/Documents/Research/Exponential Pump/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32553160-1EF7-4B28-8EA0-3BBFB24EDB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{32553160-1EF7-4B28-8EA0-3BBFB24EDB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A090F964-8CF2-4618-87DE-53654B64F8DD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{AA331077-8D97-4859-96A7-1B6D1DBCED24}"/>
   </bookViews>
@@ -36,23 +36,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>NUM STEPS</t>
   </si>
   <si>
-    <t>Hour #</t>
-  </si>
-  <si>
     <t>Speed (RPM)</t>
+  </si>
+  <si>
+    <t>Elapsed Runtime (seconds)</t>
+  </si>
+  <si>
+    <t>Min Flow Rate (RPM</t>
+  </si>
+  <si>
+    <t>Max Flow Rate (RPM)</t>
+  </si>
+  <si>
+    <t>Offset Voltage (mV)</t>
+  </si>
+  <si>
+    <t>RAW_STEPS</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>Step Duration (seconds)</t>
+  </si>
+  <si>
+    <t>Sequence (copy this --&gt;)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="hh:mm:ss"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -80,9 +115,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,111 +459,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EBF175-F5CC-4C53-A49E-A448CC5E178C}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>2.7</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>2.8</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <f>A3+H2</f>
+        <v>30</v>
+      </c>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>2.9</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>400</v>
+      </c>
+      <c r="H4">
+        <f>A4+H3</f>
+        <v>60</v>
+      </c>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>3.2</v>
-      </c>
+        <v>2.7</v>
+      </c>
+      <c r="H5">
+        <f>A5+H4</f>
+        <v>90</v>
+      </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>3.5</v>
-      </c>
+        <v>2.8</v>
+      </c>
+      <c r="H6">
+        <f>A6+H5</f>
+        <v>120</v>
+      </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>2.9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>COUNT(A2:A10000)</f>
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>3.8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
+      <c r="H7">
+        <f>A7+H6</f>
+        <v>150</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>2.9</v>
-      </c>
-      <c r="E8">
-        <f>COUNT(A:A)</f>
-        <v>8</v>
-      </c>
-      <c r="G8" t="e">
-        <f>_xlfn.TEXTJOIN(",","TRUE",$A1:B)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I8" t="e">
-        <f>_xlfn.CONCAT("&lt;",E8,",",G8,"&gt;")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I10">
-        <f>SUM(A$2:B$2,)</f>
-        <v>3.7</v>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="str">
+        <f>_xlfn.TEXTJOIN(",","TRUE",A2:B10000)</f>
+        <v>30,2.7,30,2.8,30,2.9,30,2.7,30,2.8,30,2.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="str">
+        <f>_xlfn.CONCAT("&lt;",E2,",",E3,",",E4,",",E7,",",E10,"&gt;")</f>
+        <v>&lt;2.0,5.0,400,6,30,2.7,30,2.8,30,2.9,30,2.7,30,2.8,30,2.9&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>